<commit_message>
american binomial use int
</commit_message>
<xml_diff>
--- a/xls/carr_madan.xlsx
+++ b/xls/carr_madan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keith\source\repos\Spring2023\xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kal\source\repos\FRE6233\Spring2023\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E23FC47-F30C-4E4B-8CA5-884C6779ADDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61BE6D6-AD3C-4BC9-ABA8-10E6B68A940E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="26145" windowHeight="11835" xr2:uid="{7A917F0C-3FCF-4519-84D3-59EB08CD73A5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{7A917F0C-3FCF-4519-84D3-59EB08CD73A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Value" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>s</t>
   </si>
@@ -109,9 +109,6 @@
     <t>s^2</t>
   </si>
   <si>
-    <t>=CARR_MADAN.VALUE(f0, k0, c10#, ...)</t>
-  </si>
-  <si>
     <t>fit</t>
   </si>
   <si>
@@ -123,7 +120,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -178,7 +175,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,7 +492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A977892C-3064-4E6A-9E9E-06DC0414C97A}">
   <dimension ref="A1:I542"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -568,8 +565,9 @@
       <c r="E7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>12</v>
+      <c r="F7" s="4" cm="1">
+        <f t="array" ref="F7">_xll.CARR_MADAN.VALUE(f0, k0,_xlfn.ANCHORARRAY( C10),_xlfn.ANCHORARRAY( D10), k,_xlfn.ANCHORARRAY( E10))</f>
+        <v>1.0017174610636899E-2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -586,10 +584,10 @@
         <v>7</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>